<commit_message>
Update to the Availability Excel
</commit_message>
<xml_diff>
--- a/Availability.xlsx
+++ b/Availability.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kilianleemann/Documents/HSG/Master/MLE/3_Semester/Programming with Advanced Computer Languages/Project/hsg-workplanapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347CBFC4-EF69-A14E-A286-0E118E9788F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E1C9B2-2D9A-4E4F-9F50-294B1E47B75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{687A566E-9070-F143-8DF5-DB9B81D5A7DC}"/>
   </bookViews>
@@ -851,7 +851,7 @@
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1504,7 +1504,7 @@
         <v>1</v>
       </c>
       <c r="V10" s="24">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
@@ -1589,6 +1589,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010017C71A42271A274DA461E095D9401325" ma:contentTypeVersion="8" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="30aafbe8ec0b55f3bf6040fa90919087">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f9853051-2fc0-46db-a70f-64559884f8a6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e6cc360300f9f06ae66523ed34dd87d6" ns2:_="">
     <xsd:import namespace="f9853051-2fc0-46db-a70f-64559884f8a6"/>
@@ -1758,22 +1773,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C33A2374-AF59-47C8-B91C-EBD14FA4FF35}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="f9853051-2fc0-46db-a70f-64559884f8a6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5593E7EE-975F-4520-932F-F8B899ECF7FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BD8097E-75D2-4018-98EC-DD12A33F35A9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1789,28 +1813,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5593E7EE-975F-4520-932F-F8B899ECF7FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C33A2374-AF59-47C8-B91C-EBD14FA4FF35}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="f9853051-2fc0-46db-a70f-64559884f8a6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>